<commit_message>
Gantt organisation + fix mdp user
</commit_message>
<xml_diff>
--- a/Documentation/Ecrit/01b_Diagramme_de_Gantt.xlsx
+++ b/Documentation/Ecrit/01b_Diagramme_de_Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/217fb073e6d8a319/Fichiers/Cours/BTS02_Efficom_2019_2020/Projet_BTS/M2L_R2S/Documentation/Ecrit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_80D462172F5B4425D945EF521484D17E7B1EEE66" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E39014FF-602E-418E-97DD-2ACB358879FF}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_80D462172F5B4425D945EF521484D17E7B1EEE66" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{796A8183-B014-499A-9186-C9D64CE3C064}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template GANTT Chart" sheetId="1" r:id="rId1"/>
@@ -599,10 +599,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,7 +670,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -722,7 +722,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -930,7 +930,7 @@
   <dimension ref="A1:AK1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -974,7 +974,7 @@
       </c>
       <c r="F1" s="5">
         <f ca="1">TODAY()</f>
-        <v>43903</v>
+        <v>43907</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="7"/>
@@ -1173,7 +1173,7 @@
       <c r="G3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="56">
         <f>$E$3</f>
         <v>100</v>
       </c>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="E6" s="29">
         <f>(E7+E8)/2</f>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="17" t="s">
@@ -1336,14 +1336,14 @@
       <c r="H6" s="52"/>
       <c r="I6" s="52"/>
       <c r="J6" s="52"/>
-      <c r="K6" s="56">
+      <c r="K6" s="57">
         <f>E6</f>
-        <v>100</v>
+        <v>1</v>
       </c>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
       <c r="P6" s="52"/>
       <c r="Q6" s="52"/>
       <c r="R6" s="52"/>
@@ -1380,7 +1380,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>33</v>
@@ -1391,14 +1391,14 @@
       <c r="H7" s="52"/>
       <c r="I7" s="52"/>
       <c r="J7" s="52"/>
-      <c r="K7" s="56">
+      <c r="K7" s="57">
         <f>$E$7</f>
-        <v>100</v>
+        <v>1</v>
       </c>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
       <c r="P7" s="52"/>
       <c r="Q7" s="52"/>
       <c r="R7" s="52"/>
@@ -1435,7 +1435,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>33</v>
@@ -1446,14 +1446,14 @@
       <c r="H8" s="52"/>
       <c r="I8" s="52"/>
       <c r="J8" s="52"/>
-      <c r="K8" s="56">
+      <c r="K8" s="57">
         <f>$E$8</f>
-        <v>100</v>
+        <v>1</v>
       </c>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
       <c r="P8" s="52"/>
       <c r="Q8" s="52"/>
       <c r="R8" s="52"/>
@@ -1491,23 +1491,23 @@
       </c>
       <c r="E9" s="15">
         <f>(E10+E11+E12+E13+E14)/5</f>
-        <v>100</v>
+        <v>60.4</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="56">
+      <c r="H9" s="57">
         <f>E9</f>
-        <v>100</v>
+        <v>60.4</v>
       </c>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="56"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="57"/>
       <c r="P9" s="52"/>
       <c r="Q9" s="52"/>
       <c r="R9" s="52"/>
@@ -1709,10 +1709,10 @@
         <v>28</v>
       </c>
       <c r="E13" s="25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>12</v>
@@ -1721,13 +1721,13 @@
       <c r="I13" s="52"/>
       <c r="J13" s="52"/>
       <c r="K13" s="52"/>
-      <c r="L13" s="56">
+      <c r="L13" s="57">
         <f>E13</f>
-        <v>100</v>
+        <v>1</v>
       </c>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
       <c r="P13" s="52"/>
       <c r="Q13" s="52"/>
       <c r="R13" s="52"/>
@@ -1764,7 +1764,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>33</v>
@@ -1776,13 +1776,13 @@
       <c r="I14" s="52"/>
       <c r="J14" s="52"/>
       <c r="K14" s="52"/>
-      <c r="L14" s="56">
+      <c r="L14" s="57">
         <f>E14</f>
-        <v>100</v>
+        <v>1</v>
       </c>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="56"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="57"/>
       <c r="P14" s="52"/>
       <c r="Q14" s="52"/>
       <c r="R14" s="52"/>
@@ -1820,22 +1820,22 @@
       </c>
       <c r="E15" s="37">
         <f>(E16+E17+E18+E19)/4</f>
-        <v>100</v>
+        <v>50.5</v>
       </c>
       <c r="F15" s="38"/>
       <c r="G15" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="56">
+      <c r="I15" s="57">
         <f>$E$15</f>
-        <v>100</v>
+        <v>50.5</v>
       </c>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
       <c r="P15" s="52"/>
       <c r="Q15" s="52"/>
       <c r="R15" s="52"/>
@@ -1883,13 +1883,13 @@
         <v>14</v>
       </c>
       <c r="H16" s="52"/>
-      <c r="I16" s="56">
+      <c r="I16" s="57">
         <f>$E$16</f>
         <v>100</v>
       </c>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
       <c r="M16" s="52"/>
       <c r="N16" s="52"/>
       <c r="O16" s="52"/>
@@ -1938,11 +1938,11 @@
         <v>14</v>
       </c>
       <c r="H17" s="52"/>
-      <c r="I17" s="56">
+      <c r="I17" s="57">
         <f>$E$17</f>
         <v>100</v>
       </c>
-      <c r="J17" s="56"/>
+      <c r="J17" s="57"/>
       <c r="K17" s="52"/>
       <c r="L17" s="52"/>
       <c r="M17" s="52"/>
@@ -1984,10 +1984,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G18" s="26" t="s">
         <v>14</v>
@@ -1997,11 +1997,11 @@
       <c r="J18" s="52"/>
       <c r="K18" s="52"/>
       <c r="L18" s="52"/>
-      <c r="M18" s="56">
+      <c r="M18" s="57">
         <f>$E$18</f>
-        <v>100</v>
+        <v>1</v>
       </c>
-      <c r="N18" s="56"/>
+      <c r="N18" s="57"/>
       <c r="O18" s="52"/>
       <c r="P18" s="52"/>
       <c r="Q18" s="52"/>
@@ -2039,7 +2039,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>37</v>
@@ -2056,14 +2056,14 @@
       <c r="N19" s="52"/>
       <c r="O19" s="52">
         <f>E19</f>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="P19" s="52"/>
       <c r="Q19" s="52"/>
       <c r="R19" s="52"/>
       <c r="S19" s="52"/>
-      <c r="T19" s="56"/>
-      <c r="U19" s="56"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
       <c r="V19" s="52"/>
       <c r="W19" s="52"/>
       <c r="Z19" s="51"/>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="E20" s="37">
         <f>(E21)/1</f>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="54" t="s">
@@ -2109,7 +2109,7 @@
       <c r="O20" s="52"/>
       <c r="P20" s="55">
         <f>E20</f>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="52"/>
       <c r="R20" s="52"/>
@@ -2148,10 +2148,10 @@
         <v>7</v>
       </c>
       <c r="E21" s="25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G21" s="53" t="s">
         <v>35</v>
@@ -2166,7 +2166,7 @@
       <c r="O21" s="52"/>
       <c r="P21" s="52">
         <f>E21</f>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="52"/>
       <c r="R21" s="52"/>
@@ -39373,6 +39373,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="M18:N18"/>
     <mergeCell ref="I15:O15"/>
     <mergeCell ref="H9:O9"/>
     <mergeCell ref="K7:O7"/>
@@ -39380,10 +39384,6 @@
     <mergeCell ref="K6:O6"/>
     <mergeCell ref="L13:O13"/>
     <mergeCell ref="L14:O14"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="M18:N18"/>
   </mergeCells>
   <conditionalFormatting sqref="Z4:Z21">
     <cfRule type="dataBar" priority="41">

</xml_diff>

<commit_message>
Doc fonctionnel et technique + diagram sequence
</commit_message>
<xml_diff>
--- a/Documentation/Ecrit/01b_Diagramme_de_Gantt.xlsx
+++ b/Documentation/Ecrit/01b_Diagramme_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/217fb073e6d8a319/Fichiers/Cours/BTS02_Efficom_2019_2020/Projet_BTS/M2L_R2S/Documentation/Ecrit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_80D462172F5B4425D945EF521484D17E7B1EEE66" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{796A8183-B014-499A-9186-C9D64CE3C064}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_80D462172F5B4425D945EF521484D17E7B1EEE66" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5905E4A8-DA8A-4617-BA92-B916E602B71D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,7 +930,7 @@
   <dimension ref="A1:AK1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="E6" s="29">
         <f>(E7+E8)/2</f>
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="17" t="s">
@@ -1338,7 +1338,7 @@
       <c r="J6" s="52"/>
       <c r="K6" s="57">
         <f>E6</f>
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="L6" s="57"/>
       <c r="M6" s="57"/>
@@ -1380,7 +1380,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="25">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>33</v>
@@ -1393,7 +1393,7 @@
       <c r="J7" s="52"/>
       <c r="K7" s="57">
         <f>$E$7</f>
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="L7" s="57"/>
       <c r="M7" s="57"/>
@@ -1435,7 +1435,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="25">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>33</v>
@@ -1448,7 +1448,7 @@
       <c r="J8" s="52"/>
       <c r="K8" s="57">
         <f>$E$8</f>
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="L8" s="57"/>
       <c r="M8" s="57"/>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E9" s="15">
         <f>(E10+E11+E12+E13+E14)/5</f>
-        <v>60.4</v>
+        <v>80.2</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17" t="s">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="H9" s="57">
         <f>E9</f>
-        <v>60.4</v>
+        <v>80.2</v>
       </c>
       <c r="I9" s="57"/>
       <c r="J9" s="57"/>
@@ -1764,7 +1764,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="25">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>33</v>
@@ -1778,7 +1778,7 @@
       <c r="K14" s="52"/>
       <c r="L14" s="57">
         <f>E14</f>
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="M14" s="57"/>
       <c r="N14" s="57"/>
@@ -39373,17 +39373,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="H9:O9"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="L13:O13"/>
     <mergeCell ref="T19:U19"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="I16:L16"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="I15:O15"/>
-    <mergeCell ref="H9:O9"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="L14:O14"/>
   </mergeCells>
   <conditionalFormatting sqref="Z4:Z21">
     <cfRule type="dataBar" priority="41">

</xml_diff>